<commit_message>
DataModel rewrite, PHRS Functionality, etc
</commit_message>
<xml_diff>
--- a/temp/pages/StructureDefinition-Environmental.xlsx
+++ b/temp/pages/StructureDefinition-Environmental.xlsx
@@ -54,7 +54,7 @@
     <t>Date</t>
   </si>
   <si>
-    <t>2022-03-09T09:27:10-06:00</t>
+    <t>2022-03-27T18:16:54-05:00</t>
   </si>
   <si>
     <t>Publisher</t>
@@ -72,7 +72,7 @@
     <t>Description</t>
   </si>
   <si>
-    <t>An example profile of the Environmental resource.</t>
+    <t>Standard PHR profile of the Environmental resource.</t>
   </si>
   <si>
     <t>Purpose</t>

</xml_diff>